<commit_message>
new files for demo
</commit_message>
<xml_diff>
--- a/MigrationTool/MigrationTool/Files/Applications.xlsx
+++ b/MigrationTool/MigrationTool/Files/Applications.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rajesh\Projects\MigrationTool\Publish\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rajesh\Projects\MigrationTool\MigrationTool\MigrationTool\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD328E09-3C2F-4664-B86F-FD5D50A8FC9A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{036A9151-382D-4E5E-A30F-DEC33C1384D0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8E4DB525-7351-4382-83A4-C967B7373505}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{8E4DB525-7351-4382-83A4-C967B7373505}"/>
   </bookViews>
   <sheets>
     <sheet name="Applications" sheetId="3" r:id="rId1"/>
@@ -439,7 +439,7 @@
   <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>